<commit_message>
ProjectX without DB Connections
</commit_message>
<xml_diff>
--- a/src/main/resources/datadictionary/bral.2.3.0.dd.xlsx
+++ b/src/main/resources/datadictionary/bral.2.3.0.dd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gitanshgumpu/GitHub/SpringProject/src/main/resources/datadictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903C6F63-3B30-7745-B294-23AC199B12B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A0048E-F3F2-5247-9F9C-6436399503C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1381,7 +1381,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1390,12 +1390,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1403,11 +1415,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1416,10 +1443,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1764,15 +1799,25 @@
   <dimension ref="A1:N136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="102.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="55.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.33203125" style="1" customWidth="1"/>
-    <col min="11" max="13" width="102.33203125" style="1"/>
+    <col min="7" max="7" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="102.33203125" style="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -1856,39 +1901,41 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:14" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
+      <c r="H4" s="7">
+        <v>1</v>
+      </c>
+      <c r="I4" s="7">
         <v>140</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
@@ -1907,14 +1954,16 @@
       <c r="F5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>34</v>
       </c>
@@ -1933,20 +1982,22 @@
       <c r="F6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
+      <c r="H6" s="5">
+        <v>1</v>
+      </c>
+      <c r="I6" s="5">
         <v>35</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>40</v>
       </c>
@@ -1965,27 +2016,28 @@
       <c r="F7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
+      <c r="H7" s="5">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5">
         <v>35</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="5"/>
       <c r="D8" s="5">
         <v>0</v>
       </c>
@@ -1995,27 +2047,28 @@
       <c r="F8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
+      <c r="H8" s="5">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5">
         <v>140</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="5"/>
       <c r="D9" s="5">
         <v>1</v>
       </c>
@@ -2025,214 +2078,244 @@
       <c r="F9" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:14" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="F10" s="4"/>
+      <c r="K10" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L10" s="4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="M10" s="4"/>
+    </row>
+    <row r="11" spans="1:14" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="F11" s="4"/>
+      <c r="K11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L11" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" ht="96" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="1:14" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="5">
         <v>0</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
+      <c r="H12" s="5">
+        <v>1</v>
+      </c>
+      <c r="I12" s="5">
         <v>8</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:14" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="5">
         <v>0</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="E13" s="5">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="144" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:14" s="9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D14" s="9">
+        <v>1</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="9">
         <v>4</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:14" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="F15" s="8"/>
+      <c r="K15" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="L15" s="8" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="M15" s="8"/>
+    </row>
+    <row r="16" spans="1:14" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="F16" s="8"/>
+      <c r="K16" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="L16" s="8" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" ht="112" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="1:14" s="9" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="F17" s="8"/>
+      <c r="K17" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="L17" s="8" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="1:14" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="F18" s="8"/>
+      <c r="K18" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="L18" s="8" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="M18" s="8"/>
+    </row>
+    <row r="19" spans="1:14" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="F19" s="8"/>
+      <c r="K19" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="L19" s="8" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="M19" s="8"/>
+    </row>
+    <row r="20" spans="1:14" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="F20" s="8"/>
+      <c r="K20" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="L20" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="M20" s="8"/>
+    </row>
+    <row r="21" spans="1:14" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="F21" s="8"/>
+      <c r="K21" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="L21" s="8" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="M21" s="8"/>
+    </row>
+    <row r="22" spans="1:14" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="F22" s="8"/>
+      <c r="K22" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="L22" s="8" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="M22" s="8"/>
+    </row>
+    <row r="23" spans="1:14" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="F23" s="8"/>
+      <c r="K23" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="L23" s="8" t="s">
         <v>102</v>
       </c>
+      <c r="M23" s="8"/>
     </row>
     <row r="24" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
@@ -2260,7 +2343,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="96" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>108</v>
       </c>
@@ -2271,7 +2354,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>111</v>
       </c>
@@ -2282,7 +2365,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="112" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>114</v>
       </c>
@@ -2293,7 +2376,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>117</v>
       </c>
@@ -2304,7 +2387,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>120</v>
       </c>
@@ -2315,7 +2398,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>123</v>
       </c>
@@ -2326,7 +2409,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>126</v>
       </c>
@@ -2337,7 +2420,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="96" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>129</v>
       </c>
@@ -2348,7 +2431,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>132</v>
       </c>
@@ -2359,7 +2442,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>135</v>
       </c>
@@ -2370,7 +2453,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>138</v>
       </c>
@@ -2381,7 +2464,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>141</v>
       </c>
@@ -2392,7 +2475,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>144</v>
       </c>
@@ -2403,7 +2486,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>147</v>
       </c>
@@ -2414,7 +2497,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>150</v>
       </c>
@@ -2425,7 +2508,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>153</v>
       </c>
@@ -2436,7 +2519,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>156</v>
       </c>
@@ -2447,7 +2530,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>159</v>
       </c>
@@ -2458,7 +2541,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>162</v>
       </c>
@@ -2469,7 +2552,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="96" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>165</v>
       </c>
@@ -2480,7 +2563,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>167</v>
       </c>
@@ -2491,7 +2574,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>170</v>
       </c>
@@ -2502,7 +2585,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>173</v>
       </c>
@@ -2513,7 +2596,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>176</v>
       </c>
@@ -2524,7 +2607,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>179</v>
       </c>
@@ -2535,7 +2618,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>182</v>
       </c>
@@ -2546,7 +2629,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>185</v>
       </c>
@@ -2557,7 +2640,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>188</v>
       </c>
@@ -2568,7 +2651,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>191</v>
       </c>
@@ -2594,7 +2677,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>196</v>
       </c>
@@ -2605,7 +2688,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>199</v>
       </c>
@@ -2616,7 +2699,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>202</v>
       </c>
@@ -2627,7 +2710,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="160" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>205</v>
       </c>
@@ -2638,7 +2721,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>208</v>
       </c>
@@ -2649,7 +2732,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>211</v>
       </c>
@@ -2660,7 +2743,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>214</v>
       </c>
@@ -2671,7 +2754,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>217</v>
       </c>
@@ -2682,7 +2765,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="96" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>220</v>
       </c>
@@ -2693,7 +2776,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>222</v>
       </c>
@@ -2704,7 +2787,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>225</v>
       </c>
@@ -2733,7 +2816,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>229</v>
       </c>
@@ -2756,7 +2839,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>234</v>
       </c>
@@ -2788,7 +2871,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>240</v>
       </c>
@@ -2846,7 +2929,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>248</v>
       </c>
@@ -2869,7 +2952,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>252</v>
       </c>
@@ -2901,7 +2984,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>253</v>
       </c>
@@ -2930,7 +3013,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>254</v>
       </c>
@@ -2959,7 +3042,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>255</v>
       </c>
@@ -2982,7 +3065,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>259</v>
       </c>
@@ -3014,7 +3097,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>260</v>
       </c>
@@ -3072,7 +3155,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>262</v>
       </c>
@@ -3095,7 +3178,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>267</v>
       </c>
@@ -3275,7 +3358,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="256" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" ht="160" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>303</v>
       </c>
@@ -3301,7 +3384,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="256" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" ht="160" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>309</v>
       </c>
@@ -3379,7 +3462,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="80" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>319</v>
       </c>
@@ -3402,7 +3485,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="80" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>324</v>
       </c>
@@ -3425,7 +3508,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>327</v>
       </c>
@@ -3508,7 +3591,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>332</v>
       </c>
@@ -3548,7 +3631,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>337</v>
       </c>
@@ -3608,7 +3691,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="256" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:14" ht="160" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>340</v>
       </c>
@@ -3634,7 +3717,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="256" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:14" ht="160" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>341</v>
       </c>
@@ -3683,7 +3766,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>347</v>
       </c>
@@ -3783,7 +3866,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>370</v>
       </c>
@@ -3812,7 +3895,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>374</v>
       </c>
@@ -3841,7 +3924,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>378</v>
       </c>
@@ -3954,7 +4037,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>386</v>
       </c>
@@ -3980,7 +4063,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>392</v>
       </c>
@@ -4009,7 +4092,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>396</v>
       </c>
@@ -4038,7 +4121,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>400</v>
       </c>
@@ -4067,7 +4150,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>404</v>
       </c>
@@ -4125,7 +4208,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>412</v>
       </c>
@@ -4151,7 +4234,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>418</v>
       </c>
@@ -4252,7 +4335,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>439</v>
       </c>

</xml_diff>